<commit_message>
Some changes from PR not all
</commit_message>
<xml_diff>
--- a/Result_15052025.xlsx
+++ b/Result_15052025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s194351_dtu_dk/Documents/Dokumenter/Master Thesis/MasterThesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="115_{A9A1507D-7C72-44DF-AF81-3DE51B7E6770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30F29766-F2D7-4574-8E25-1EF8B6675883}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="115_{A9A1507D-7C72-44DF-AF81-3DE51B7E6770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC8D895C-BE20-44C0-8D6A-9C2A29A39BE6}"/>
   <bookViews>
-    <workbookView xWindow="-15015" yWindow="-24120" windowWidth="57840" windowHeight="23520" activeTab="2" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-15015" yWindow="-24120" windowWidth="57840" windowHeight="23520" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5129,11 +5129,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4B00FF-D5DF-4341-A74C-07E5BBC42628}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5259,7 +5258,7 @@
         <v>3.8569999999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>326</v>
       </c>
@@ -5377,7 +5376,7 @@
         <v>1.8079999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>326</v>
       </c>
@@ -5495,7 +5494,7 @@
         <v>-0.87199999999999989</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>326</v>
       </c>
@@ -5613,7 +5612,7 @@
         <v>-1.0895999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>326</v>
       </c>
@@ -5731,7 +5730,7 @@
         <v>3.5591999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>751</v>
       </c>
@@ -5849,7 +5848,7 @@
         <v>-2.1753999999999989</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>751</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>2.9610000000000012</v>
       </c>
     </row>
-    <row r="15" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>751</v>
       </c>
@@ -6085,7 +6084,7 @@
         <v>3.1684000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>751</v>
       </c>
@@ -6145,13 +6144,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C17" xr:uid="{CA4B00FF-D5DF-4341-A74C-07E5BBC42628}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="0.5"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C17" xr:uid="{CA4B00FF-D5DF-4341-A74C-07E5BBC42628}"/>
   <conditionalFormatting sqref="P2:P17">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -6184,7 +6177,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1F7297-E8B2-44A5-A1F2-E37784734FCC}">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>